<commit_message>
Corrección en la solicitud
Corrección en el nombre de archivo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion07/SolicitudGrafica LE_06_07_CO_REC160.xlsx
+++ b/fuentes/contenidos/grado06/guion07/SolicitudGrafica LE_06_07_CO_REC160.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\GitHub\Lenguaje\fuentes\contenidos\grado06\guion07\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -596,9 +596,6 @@
     <t>Cristian Pineda</t>
   </si>
   <si>
-    <t>LE_07_06_CO_REC160</t>
-  </si>
-  <si>
     <t>reloj</t>
   </si>
   <si>
@@ -618,6 +615,9 @@
   </si>
   <si>
     <t>Fotografía</t>
+  </si>
+  <si>
+    <t>LE_06_07_CO_REC160</t>
   </si>
 </sst>
 </file>
@@ -2495,7 +2495,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2693,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -2796,14 +2796,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_07_06_CO_REC160_IMG01.png</v>
+        <v>LE_06_07_CO_REC160_IMG01.png</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2818,7 +2818,7 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -2839,14 +2839,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_07_06_CO_REC160_IMG02.png</v>
+        <v>LE_06_07_CO_REC160_IMG02.png</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2861,7 +2861,7 @@
         <v/>
       </c>
       <c r="J11" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K11" s="65"/>
       <c r="O11" s="2" t="str">
@@ -2882,14 +2882,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_07_06_CO_REC160_IMG03.png</v>
+        <v>LE_06_07_CO_REC160_IMG03.png</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2904,7 +2904,7 @@
         <v/>
       </c>
       <c r="J12" s="64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -2925,14 +2925,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_07_06_CO_REC160_IMG04.png</v>
+        <v>LE_06_07_CO_REC160_IMG04.png</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2947,7 +2947,7 @@
         <v/>
       </c>
       <c r="J13" s="64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
@@ -2968,14 +2968,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_07_06_CO_REC160_IMG05.png</v>
+        <v>LE_06_07_CO_REC160_IMG05.png</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2990,7 +2990,7 @@
         <v/>
       </c>
       <c r="J14" s="64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
@@ -3011,14 +3011,14 @@
         <v>Recurso M3A</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E15" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_07_06_CO_REC160_IMG06.png</v>
+        <v>LE_06_07_CO_REC160_IMG06.png</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3033,7 +3033,7 @@
         <v/>
       </c>
       <c r="J15" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">

</xml_diff>